<commit_message>
Excel file updated with invalid data
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B52\Workspace\actitime\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86AFD0E-0615-408A-8364-69A17BC2CC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16665" windowHeight="6615"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="validLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,24 +26,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>username</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
   <si>
     <t>manager</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>admin</t>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -341,18 +353,52 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC1DFA0-95CC-4A7A-8097-F0939627E15C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -362,15 +408,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>